<commit_message>
Fixing Lily's bug: directions are now not counted as a date.
</commit_message>
<xml_diff>
--- a/CRM_BVI/database/directions.xlsx
+++ b/CRM_BVI/database/directions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -67,6 +67,18 @@
     <t xml:space="preserve">✓ </t>
   </si>
   <si>
+    <t xml:space="preserve">24.05.07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.03.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.03.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.03.02</t>
+  </si>
+  <si>
     <t xml:space="preserve">38.03.02</t>
   </si>
   <si>
@@ -74,6 +86,15 @@
   </si>
   <si>
     <t xml:space="preserve">Копия</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.03.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09.03.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.03.02</t>
   </si>
 </sst>
 </file>
@@ -82,7 +103,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -201,10 +222,10 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="M7" activeCellId="0" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.47265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48828125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.3"/>
@@ -278,20 +299,20 @@
       <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="n">
-        <v>39226</v>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>36963</v>
-      </c>
-      <c r="K2" s="3" t="n">
-        <v>37324</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>36960</v>
-      </c>
-      <c r="M2" s="0" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,7 +323,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>258</v>
@@ -311,17 +332,19 @@
         <v>253</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="3" t="n">
-        <v>37316</v>
-      </c>
-      <c r="J3" s="3" t="n">
-        <v>38055</v>
-      </c>
-      <c r="K3" s="3" t="n">
-        <v>37317</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>